<commit_message>
Block diagram for poster.
</commit_message>
<xml_diff>
--- a/Documentation/Test plan.xlsx
+++ b/Documentation/Test plan.xlsx
@@ -11,13 +11,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$18:$D$18</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$2:$D$76</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="100">
   <si>
     <t>Device:</t>
   </si>
@@ -762,8 +763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:G76"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B77" sqref="B77"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G73" sqref="G73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1146,10 +1147,12 @@
       <c r="B45" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C45" s="10" t="s">
+      <c r="C45" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D45" s="8"/>
+      <c r="D45" s="8" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="46" spans="2:4">
       <c r="B46" s="11" t="s">
@@ -1173,7 +1176,7 @@
       <c r="B48" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C48" s="10" t="s">
+      <c r="C48" s="13" t="s">
         <v>55</v>
       </c>
       <c r="D48" s="8"/>
@@ -1200,7 +1203,7 @@
       <c r="B51" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C51" s="10" t="s">
+      <c r="C51" s="13" t="s">
         <v>55</v>
       </c>
       <c r="D51" s="8"/>
@@ -1236,7 +1239,7 @@
       <c r="B55" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="C55" s="10" t="s">
+      <c r="C55" s="13" t="s">
         <v>55</v>
       </c>
       <c r="D55" s="8"/>
@@ -1279,10 +1282,12 @@
       <c r="B60" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C60" s="10" t="s">
+      <c r="C60" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D60" s="8"/>
+      <c r="D60" s="8" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="61" spans="2:4">
       <c r="B61" s="11" t="s">
@@ -1306,7 +1311,7 @@
       <c r="B63" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="C63" s="10" t="s">
+      <c r="C63" s="13" t="s">
         <v>55</v>
       </c>
       <c r="D63" s="8"/>
@@ -1333,7 +1338,7 @@
       <c r="B66" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C66" s="10" t="s">
+      <c r="C66" s="13" t="s">
         <v>55</v>
       </c>
       <c r="D66" s="8"/>
@@ -1360,7 +1365,7 @@
       <c r="B69" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="C69" s="10" t="s">
+      <c r="C69" s="13" t="s">
         <v>55</v>
       </c>
       <c r="D69" s="8"/>
@@ -1396,7 +1401,7 @@
       <c r="B73" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="C73" s="10" t="s">
+      <c r="C73" s="13" t="s">
         <v>55</v>
       </c>
       <c r="D73" s="8"/>

</xml_diff>